<commit_message>
NN-676 #time 1h feature: resolved bdd issues
</commit_message>
<xml_diff>
--- a/test/support/ValidSheet.xlsx
+++ b/test/support/ValidSheet.xlsx
@@ -154,8 +154,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -251,163 +255,163 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
NN-103 #time feature: G2P uploade issue is solved
</commit_message>
<xml_diff>
--- a/test/support/ValidSheet.xlsx
+++ b/test/support/ValidSheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">SL No</t>
   </si>
@@ -43,22 +43,13 @@
     <t xml:space="preserve">Ajeeb Bin HAMID</t>
   </si>
   <si>
-    <t xml:space="preserve">AGT234815</t>
+    <t xml:space="preserve">CMR15019448</t>
   </si>
   <si>
     <t xml:space="preserve">265 46 419 2496</t>
   </si>
   <si>
     <t xml:space="preserve">BDD TESTING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gunner August JAST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGT814116</t>
-  </si>
-  <si>
-    <t xml:space="preserve">265 10 534 1679</t>
   </si>
 </sst>
 </file>
@@ -255,10 +246,10 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -301,24 +292,12 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">

</xml_diff>

<commit_message>
NN-542 #time 3h feature:completed google ap integration and resolved g2p trasaction issue and delete account page number issue
</commit_message>
<xml_diff>
--- a/test/support/ValidSheet.xlsx
+++ b/test/support/ValidSheet.xlsx
@@ -246,10 +246,10 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -285,7 +285,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
NN-368 #time 10m feature:Paymaart - Admin Web- Insights of Merchant Registration BDD issue solved.
</commit_message>
<xml_diff>
--- a/test/support/ValidSheet.xlsx
+++ b/test/support/ValidSheet.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -43,10 +43,10 @@
     <t xml:space="preserve">Ajeeb Bin HAMID</t>
   </si>
   <si>
-    <t xml:space="preserve">CMR15019448</t>
-  </si>
-  <si>
-    <t xml:space="preserve">265 46 419 2496</t>
+    <t xml:space="preserve">CMR47857280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">265 84 546 3484 </t>
   </si>
   <si>
     <t xml:space="preserve">BDD TESTING</t>
@@ -150,19 +150,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -238,20 +238,126 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -271,7 +377,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -291,7 +397,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>

</xml_diff>

<commit_message>
NN-368 #time 5m feature:Paymaart - Admin Web- Insights of Merchant Registration BDD issue solved.
</commit_message>
<xml_diff>
--- a/test/support/ValidSheet.xlsx
+++ b/test/support/ValidSheet.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -43,10 +43,10 @@
     <t xml:space="preserve">Ajeeb Bin HAMID</t>
   </si>
   <si>
-    <t xml:space="preserve">CMR47857280</t>
-  </si>
-  <si>
-    <t xml:space="preserve">265 84 546 3484 </t>
+    <t xml:space="preserve">CMR15019448</t>
+  </si>
+  <si>
+    <t xml:space="preserve">265 46 419 2496</t>
   </si>
   <si>
     <t xml:space="preserve">BDD TESTING</t>
@@ -150,19 +150,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -238,126 +238,20 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -377,7 +271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -397,7 +291,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>

</xml_diff>